<commit_message>
Resolvendo o problema do relátorio
</commit_message>
<xml_diff>
--- a/N1.xlsx
+++ b/N1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Nome</t>
   </si>
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>Data de Nascimento</t>
-  </si>
-  <si>
-    <t>Kaka</t>
   </si>
   <si>
     <t>Fernando</t>
@@ -38,9 +35,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -94,13 +90,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -416,22 +411,11 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>123</v>
+      <c r="B2" t="s">
+        <v>4</v>
       </c>
       <c r="C2" s="2">
-        <v>34619</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3">
-        <v>38216</v>
+        <v>37120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tratamento de erros pt1
Tratando algumas exceções do programa.
</commit_message>
<xml_diff>
--- a/N1.xlsx
+++ b/N1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Nome</t>
   </si>
@@ -26,14 +26,24 @@
   </si>
   <si>
     <t>Fernando</t>
+  </si>
+  <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>158</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -87,12 +97,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -408,10 +419,21 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>154</v>
+      <c r="B2" t="s">
+        <v>5</v>
       </c>
       <c r="C2" s="2">
+        <v>37120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
         <v>37120</v>
       </c>
     </row>

</xml_diff>